<commit_message>
Single core single client postgres data
</commit_message>
<xml_diff>
--- a/postgres.xlsx
+++ b/postgres.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="24820" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="24680" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1GB" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="72">
   <si>
     <t>CPU_CLK_UNHALTED.THREAD_P</t>
   </si>
@@ -215,25 +215,37 @@
     <t>total (7000000)</t>
   </si>
   <si>
-    <t>baseline</t>
-  </si>
-  <si>
-    <t>force 2M alignment of libraries</t>
-  </si>
-  <si>
-    <t>shared PTPs</t>
-  </si>
-  <si>
-    <t>1G 2j</t>
-  </si>
-  <si>
-    <t>1G 1j</t>
-  </si>
-  <si>
     <t>force/base</t>
   </si>
   <si>
     <t>shared/base</t>
+  </si>
+  <si>
+    <t>Ms_L</t>
+  </si>
+  <si>
+    <t>Ms_Lf</t>
+  </si>
+  <si>
+    <t>Mst_Lt</t>
+  </si>
+  <si>
+    <t>2 cores, 2 clients, 1G</t>
+  </si>
+  <si>
+    <t>Re-run 2 cores, 2 clients, 1G</t>
+  </si>
+  <si>
+    <t>1 core, 1 client, 1G</t>
+  </si>
+  <si>
+    <t>Run 1</t>
+  </si>
+  <si>
+    <t>Run 2</t>
+  </si>
+  <si>
+    <t>Run 3</t>
   </si>
 </sst>
 </file>
@@ -321,7 +333,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1"/>
@@ -337,6 +349,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="5" builtinId="3"/>
@@ -2180,10 +2193,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2199,48 +2212,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>64</v>
       </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10" t="s">
+      <c r="J2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="A3" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -2248,30 +2261,30 @@
         <v>0</v>
       </c>
       <c r="B4" s="7">
-        <v>146984.773464</v>
+        <v>140403.96484500001</v>
       </c>
       <c r="C4" s="1">
-        <v>1175878187712</v>
+        <v>1123231718763.5</v>
       </c>
       <c r="D4" s="7">
-        <v>152389.60000899999</v>
+        <v>145435.15202400001</v>
       </c>
       <c r="E4" s="1">
-        <v>1219116800073.5</v>
+        <v>1163481216192.5</v>
       </c>
       <c r="F4" s="7">
-        <v>146428.94732499999</v>
+        <v>140926.72194799999</v>
       </c>
       <c r="G4" s="1">
-        <v>1171431578603.5</v>
+        <v>1127413775585.5</v>
       </c>
       <c r="I4" s="1">
-        <f>E4/C4</f>
-        <v>1.0367713363623428</v>
+        <f t="shared" ref="I4:I12" si="0">E4/C4</f>
+        <v>1.0358336545849225</v>
       </c>
       <c r="J4" s="1">
-        <f>G4/C4</f>
-        <v>0.99621847810855979</v>
+        <f t="shared" ref="J4:J12" si="1">G4/C4</f>
+        <v>1.0037232360448329</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -2279,30 +2292,30 @@
         <v>1</v>
       </c>
       <c r="B5" s="7">
-        <v>26.430181000000001</v>
+        <v>28.554079999999999</v>
       </c>
       <c r="C5" s="1">
-        <v>211441451.5</v>
+        <v>228432639.5</v>
       </c>
       <c r="D5" s="7">
-        <v>27.717406</v>
+        <v>26.626676</v>
       </c>
       <c r="E5" s="1">
-        <v>221739252</v>
+        <v>213013409</v>
       </c>
       <c r="F5" s="7">
-        <v>13.123818999999999</v>
+        <v>14.53087</v>
       </c>
       <c r="G5" s="1">
-        <v>104990555</v>
+        <v>116246957.5</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" ref="I5:I23" si="0">E5/C5</f>
-        <v>1.0487028462344812</v>
+        <f t="shared" si="0"/>
+        <v>0.93249988034218723</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" ref="J5:J23" si="1">G5/C5</f>
-        <v>0.49654670006841112</v>
+        <f t="shared" si="1"/>
+        <v>0.50888943784235352</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -2310,30 +2323,30 @@
         <v>2</v>
       </c>
       <c r="B6" s="7">
-        <v>11.123400999999999</v>
+        <v>10.944258</v>
       </c>
       <c r="C6" s="1">
-        <v>88987204</v>
+        <v>87554067</v>
       </c>
       <c r="D6" s="7">
-        <v>15.163019999999999</v>
+        <v>12.925743000000001</v>
       </c>
       <c r="E6" s="1">
-        <v>121304157</v>
+        <v>103405943</v>
       </c>
       <c r="F6" s="7">
-        <v>5.4515750000000001</v>
+        <v>5.9714359999999997</v>
       </c>
       <c r="G6" s="1">
-        <v>43612601</v>
+        <v>47771488</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
-        <v>1.3631640454733245</v>
+        <v>1.181052423298623</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="1"/>
-        <v>0.49009968893954686</v>
+        <v>0.54562271790298444</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -2341,30 +2354,30 @@
         <v>16</v>
       </c>
       <c r="B7" s="7">
-        <v>11.122903000000001</v>
+        <v>10.943394</v>
       </c>
       <c r="C7" s="1">
-        <v>88983225.5</v>
+        <v>87547152.5</v>
       </c>
       <c r="D7" s="7">
-        <v>15.163021000000001</v>
+        <v>12.925741</v>
       </c>
       <c r="E7" s="1">
-        <v>121304167.5</v>
+        <v>103405928.5</v>
       </c>
       <c r="F7" s="7">
-        <v>5.4440689999999998</v>
+        <v>5.9696889999999998</v>
       </c>
       <c r="G7" s="1">
-        <v>43552552</v>
+        <v>47757510</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>1.3632251114565408</v>
+        <v>1.1811455375433255</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="1"/>
-        <v>0.48944676657062741</v>
+        <v>0.54550614881506287</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -2378,30 +2391,30 @@
         <v>4</v>
       </c>
       <c r="B9" s="7">
-        <v>801.64434600000004</v>
+        <v>773.14375399999994</v>
       </c>
       <c r="C9" s="1">
-        <v>6413154766</v>
+        <v>6185150034.5</v>
       </c>
       <c r="D9" s="7">
-        <v>1165.3940809999999</v>
+        <v>1124.52547</v>
       </c>
       <c r="E9" s="1">
-        <v>9323152650</v>
+        <v>8996203760</v>
       </c>
       <c r="F9" s="7">
-        <v>383.13884100000001</v>
+        <v>428.18488100000002</v>
       </c>
       <c r="G9" s="1">
-        <v>3065110728.5</v>
+        <v>3425479049</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>1.4537545077545382</v>
+        <v>1.4544843229057163</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="1"/>
-        <v>0.47794117565195837</v>
+        <v>0.55382311340761381</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -2409,30 +2422,30 @@
         <v>17</v>
       </c>
       <c r="B10" s="7">
-        <v>5.2099999999999998E-4</v>
+        <v>8.1999999999999998E-4</v>
       </c>
       <c r="C10" s="1">
-        <v>4166</v>
+        <v>6562.5</v>
       </c>
       <c r="D10" s="7">
-        <v>6.9999999999999999E-6</v>
+        <v>3.9999999999999998E-6</v>
       </c>
       <c r="E10" s="1">
-        <v>52.5</v>
+        <v>35</v>
       </c>
       <c r="F10" s="7">
-        <v>2.9979999999999998E-3</v>
+        <v>1.4607999999999999E-2</v>
       </c>
       <c r="G10" s="1">
-        <v>23981.5</v>
+        <v>116865.5</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>1.2602016322611619E-2</v>
+        <v>5.3333333333333332E-3</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="1"/>
-        <v>5.7564810369659147</v>
+        <v>17.808076190476189</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -2443,27 +2456,27 @@
         <v>3.0000000000000001E-6</v>
       </c>
       <c r="C11" s="1">
-        <v>20</v>
+        <v>20.5</v>
       </c>
       <c r="D11" s="7">
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="E11" s="1">
-        <v>28.5</v>
+        <v>30</v>
       </c>
       <c r="F11" s="7">
-        <v>3.9999999999999998E-6</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="G11" s="1">
-        <v>30.5</v>
+        <v>27.5</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="0"/>
-        <v>1.425</v>
+        <v>1.4634146341463414</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="1"/>
-        <v>1.5249999999999999</v>
+        <v>1.3414634146341464</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -2471,296 +2484,288 @@
         <v>3</v>
       </c>
       <c r="B12" s="7">
-        <v>46.604286000000002</v>
+        <v>50.312914999999997</v>
       </c>
       <c r="C12" s="1">
-        <v>372834289.5</v>
+        <v>402503318</v>
       </c>
       <c r="D12" s="7">
-        <v>618.88340200000005</v>
+        <v>625.74868200000003</v>
       </c>
       <c r="E12" s="1">
-        <v>4951067219</v>
+        <v>5005989457.5</v>
       </c>
       <c r="F12" s="7">
-        <v>50.313581999999997</v>
+        <v>53.105401000000001</v>
       </c>
       <c r="G12" s="1">
-        <v>402508657.5</v>
+        <v>424843206.5</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="0"/>
-        <v>13.279538278627133</v>
+        <v>12.437138362919036</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="1"/>
-        <v>1.0795913059386133</v>
+        <v>1.0555023710388396</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>65</v>
+      <c r="D14" s="1">
+        <v>140447.25551799999</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1123578044142</v>
+      </c>
+      <c r="F14" s="1">
+        <v>139853.61392999999</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1118828911444</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="D15" s="1">
+        <v>10.607939999999999</v>
+      </c>
+      <c r="E15" s="1">
+        <v>84863516.5</v>
+      </c>
+      <c r="F15" s="1">
+        <v>15.165372</v>
+      </c>
+      <c r="G15" s="1">
+        <v>121322979.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D16" s="1">
+        <v>3.6480079999999999</v>
+      </c>
+      <c r="E16" s="1">
+        <v>29184064</v>
+      </c>
+      <c r="F16" s="1">
+        <v>5.9287380000000001</v>
+      </c>
+      <c r="G16" s="1">
+        <v>47429904</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D17" s="1">
+        <v>3.6466409999999998</v>
+      </c>
+      <c r="E17" s="1">
+        <v>29173127</v>
+      </c>
+      <c r="F17" s="1">
+        <v>5.9264429999999999</v>
+      </c>
+      <c r="G17" s="1">
+        <v>47411542.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D19" s="1">
+        <v>375.49195500000002</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3003935643.5</v>
+      </c>
+      <c r="F19" s="1">
+        <v>415.12147900000002</v>
+      </c>
+      <c r="G19" s="1">
+        <v>3320971828.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D20" s="1">
+        <v>1.639E-3</v>
+      </c>
+      <c r="E20" s="1">
+        <v>13115.5</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2.1970000000000002E-3</v>
+      </c>
+      <c r="G20" s="1">
+        <v>17574.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D21" s="1">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="E21" s="1">
+        <v>30.5</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="G21" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D22" s="1">
+        <v>50.376511999999998</v>
+      </c>
+      <c r="E22" s="1">
+        <v>403012099.5</v>
+      </c>
+      <c r="F22" s="1">
+        <v>53.54824</v>
+      </c>
+      <c r="G22" s="1">
+        <v>428385921.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="7">
-        <v>140403.96484500001</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1123231718763.5</v>
-      </c>
-      <c r="D15" s="7">
-        <v>145435.15202400001</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1163481216192.5</v>
-      </c>
-      <c r="F15" s="7">
-        <v>140926.72194799999</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1127413775585.5</v>
-      </c>
-      <c r="I15" s="1">
-        <f t="shared" si="0"/>
-        <v>1.0358336545849225</v>
-      </c>
-      <c r="J15" s="1">
-        <f t="shared" si="1"/>
-        <v>1.0037232360448329</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="C26" s="1">
+        <v>877280361133</v>
+      </c>
+      <c r="E26" s="1">
+        <v>878772319920</v>
+      </c>
+      <c r="G26" s="1">
+        <v>877464443912</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="7">
-        <v>28.554079999999999</v>
-      </c>
-      <c r="C16" s="1">
-        <v>228432639.5</v>
-      </c>
-      <c r="D16" s="7">
-        <v>26.626676</v>
-      </c>
-      <c r="E16" s="1">
-        <v>213013409</v>
-      </c>
-      <c r="F16" s="7">
-        <v>14.53087</v>
-      </c>
-      <c r="G16" s="1">
-        <v>116246957.5</v>
-      </c>
-      <c r="I16" s="1">
-        <f t="shared" si="0"/>
-        <v>0.93249988034218723</v>
-      </c>
-      <c r="J16" s="1">
-        <f t="shared" si="1"/>
-        <v>0.50888943784235352</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="C27" s="1">
+        <v>210538810</v>
+      </c>
+      <c r="E27" s="1">
+        <v>356654916</v>
+      </c>
+      <c r="G27" s="1">
+        <v>195628734</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="7">
-        <v>10.944258</v>
-      </c>
-      <c r="C17" s="1">
-        <v>87554067</v>
-      </c>
-      <c r="D17" s="7">
-        <v>12.925743000000001</v>
-      </c>
-      <c r="E17" s="1">
-        <v>103405943</v>
-      </c>
-      <c r="F17" s="7">
-        <v>5.9714359999999997</v>
-      </c>
-      <c r="G17" s="1">
-        <v>47771488</v>
-      </c>
-      <c r="I17" s="1">
-        <f t="shared" si="0"/>
-        <v>1.181052423298623</v>
-      </c>
-      <c r="J17" s="1">
-        <f t="shared" si="1"/>
-        <v>0.54562271790298444</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="C28" s="1">
+        <v>123363462</v>
+      </c>
+      <c r="E28" s="1">
+        <v>228892890</v>
+      </c>
+      <c r="G28" s="1">
+        <v>119632667</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="7">
-        <v>10.943394</v>
-      </c>
-      <c r="C18" s="1">
-        <v>87547152.5</v>
-      </c>
-      <c r="D18" s="7">
-        <v>12.925741</v>
-      </c>
-      <c r="E18" s="1">
-        <v>103405928.5</v>
-      </c>
-      <c r="F18" s="7">
-        <v>5.9696889999999998</v>
-      </c>
-      <c r="G18" s="1">
-        <v>47757510</v>
-      </c>
-      <c r="I18" s="1">
-        <f t="shared" si="0"/>
-        <v>1.1811455375433255</v>
-      </c>
-      <c r="J18" s="1">
-        <f t="shared" si="1"/>
-        <v>0.54550614881506287</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="C29" s="1">
+        <v>123361377</v>
+      </c>
+      <c r="E29" s="1">
+        <v>228890858</v>
+      </c>
+      <c r="G29" s="1">
+        <v>119630592</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="7">
-        <v>773.14375399999994</v>
-      </c>
-      <c r="C20" s="1">
-        <v>6185150034.5</v>
-      </c>
-      <c r="D20" s="7">
-        <v>1124.52547</v>
-      </c>
-      <c r="E20" s="1">
-        <v>8996203760</v>
-      </c>
-      <c r="F20" s="7">
-        <v>428.18488100000002</v>
-      </c>
-      <c r="G20" s="1">
-        <v>3425479049</v>
-      </c>
-      <c r="I20" s="1">
-        <f t="shared" si="0"/>
-        <v>1.4544843229057163</v>
-      </c>
-      <c r="J20" s="1">
-        <f t="shared" si="1"/>
-        <v>0.55382311340761381</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="C31" s="1">
+        <v>6461413845</v>
+      </c>
+      <c r="E31" s="1">
+        <v>6913162471</v>
+      </c>
+      <c r="G31" s="1">
+        <v>6144949457</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="7">
-        <v>8.1999999999999998E-4</v>
-      </c>
-      <c r="C21" s="1">
-        <v>6562.5</v>
-      </c>
-      <c r="D21" s="7">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="E21" s="1">
-        <v>35</v>
-      </c>
-      <c r="F21" s="7">
-        <v>1.4607999999999999E-2</v>
-      </c>
-      <c r="G21" s="1">
-        <v>116865.5</v>
-      </c>
-      <c r="I21" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3333333333333332E-3</v>
-      </c>
-      <c r="J21" s="1">
-        <f t="shared" si="1"/>
-        <v>17.808076190476189</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="C32" s="1">
+        <v>2204</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2035</v>
+      </c>
+      <c r="G32" s="1">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="7">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="C22" s="1">
-        <v>20.5</v>
-      </c>
-      <c r="D22" s="7">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="E22" s="1">
-        <v>30</v>
-      </c>
-      <c r="F22" s="7">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="G22" s="1">
-        <v>27.5</v>
-      </c>
-      <c r="I22" s="1">
-        <f t="shared" si="0"/>
-        <v>1.4634146341463414</v>
-      </c>
-      <c r="J22" s="1">
-        <f t="shared" si="1"/>
-        <v>1.3414634146341464</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="C33" s="1">
+        <v>36</v>
+      </c>
+      <c r="E33" s="1">
+        <v>36</v>
+      </c>
+      <c r="G33" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="7">
-        <v>50.312914999999997</v>
-      </c>
-      <c r="C23" s="1">
-        <v>402503318</v>
-      </c>
-      <c r="D23" s="7">
-        <v>625.74868200000003</v>
-      </c>
-      <c r="E23" s="1">
-        <v>5005989457.5</v>
-      </c>
-      <c r="F23" s="7">
-        <v>53.105401000000001</v>
-      </c>
-      <c r="G23" s="1">
-        <v>424843206.5</v>
-      </c>
-      <c r="I23" s="1">
-        <f t="shared" si="0"/>
-        <v>12.437138362919036</v>
-      </c>
-      <c r="J23" s="1">
-        <f t="shared" si="1"/>
-        <v>1.0555023710388396</v>
+      <c r="C34" s="1">
+        <v>389807917</v>
+      </c>
+      <c r="E34" s="1">
+        <v>400868717</v>
+      </c>
+      <c r="G34" s="1">
+        <v>402446396</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Preliminary postgres code padding data
</commit_message>
<xml_diff>
--- a/postgres.xlsx
+++ b/postgres.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="89">
   <si>
     <t>CPU_CLK_UNHALTED.THREAD_P</t>
   </si>
@@ -270,6 +270,33 @@
   </si>
   <si>
     <t>LTO+PGO</t>
+  </si>
+  <si>
+    <t>pre_md</t>
+  </si>
+  <si>
+    <t>11.2-release_nopti</t>
+  </si>
+  <si>
+    <t>11.2-release_pti</t>
+  </si>
+  <si>
+    <t>1 phys core, 2 workers, 1G, select-only, linked with lld --no-rosegment and max-page-size=0x200000</t>
+  </si>
+  <si>
+    <t>What does DTLB and STLB look like? The increse here might  be from DTLB competition.</t>
+  </si>
+  <si>
+    <t>How many of these are 4K, and how many are 2M?</t>
+  </si>
+  <si>
+    <t>Ms_Lf with padding</t>
+  </si>
+  <si>
+    <t>ITLB_MISSES.STLB_HIT_4K</t>
+  </si>
+  <si>
+    <t>ITLB_MISSES.STLB_HIT_2M</t>
   </si>
 </sst>
 </file>
@@ -2217,10 +2244,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M67"/>
+  <dimension ref="A1:Q118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+    <sheetView tabSelected="1" topLeftCell="F50" workbookViewId="0">
+      <selection activeCell="L73" sqref="L73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2238,7 +2265,9 @@
     <col min="11" max="11" width="19" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.83203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="20.5" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="1"/>
+    <col min="14" max="14" width="14" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -3032,7 +3061,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>64</v>
       </c>
@@ -3046,7 +3075,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>0</v>
       </c>
@@ -3060,7 +3089,7 @@
         <v>876277641654</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>73</v>
       </c>
@@ -3074,7 +3103,7 @@
         <v>300150254</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>1</v>
       </c>
@@ -3088,7 +3117,7 @@
         <v>228684685</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>4</v>
       </c>
@@ -3102,7 +3131,7 @@
         <v>6541289608</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C54" s="1" t="s">
         <v>68</v>
       </c>
@@ -3113,7 +3142,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -3127,7 +3156,7 @@
         <v>874985735564</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>16</v>
       </c>
@@ -3141,7 +3170,7 @@
         <v>129438461</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>17</v>
       </c>
@@ -3155,7 +3184,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>3</v>
       </c>
@@ -3169,15 +3198,15 @@
         <v>398384398</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="B61" s="11" t="s">
         <v>76</v>
@@ -3197,8 +3226,10 @@
       <c r="K61" s="11"/>
       <c r="L61" s="11"/>
       <c r="M61" s="11"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N61" s="11"/>
+      <c r="O61" s="11"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B62" s="11" t="s">
         <v>75</v>
       </c>
@@ -3223,8 +3254,12 @@
         <v>64</v>
       </c>
       <c r="M62" s="11"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N62" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="O62" s="11"/>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B63" s="6" t="s">
         <v>33</v>
       </c>
@@ -3261,8 +3296,14 @@
       <c r="M63" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N63" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O63" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -3297,13 +3338,22 @@
         <v>1116639959108</v>
       </c>
       <c r="L64" s="1">
-        <v>138141.08767099999</v>
+        <v>138231.978798</v>
       </c>
       <c r="M64" s="1">
-        <v>1105128701366</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1105855830385</v>
+      </c>
+      <c r="N64" s="1">
+        <v>136578.52948699999</v>
+      </c>
+      <c r="O64" s="1">
+        <v>1092628235895</v>
+      </c>
+      <c r="Q64" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>73</v>
       </c>
@@ -3338,13 +3388,22 @@
         <v>1494074172.5</v>
       </c>
       <c r="L65" s="1">
-        <v>188.930027</v>
+        <v>186.79355100000001</v>
       </c>
       <c r="M65" s="1">
-        <v>1511440217.5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1494348410</v>
+      </c>
+      <c r="N65" s="1">
+        <v>190.30417299999999</v>
+      </c>
+      <c r="O65" s="1">
+        <v>1522433383.5</v>
+      </c>
+      <c r="Q65" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>1</v>
       </c>
@@ -3379,15 +3438,24 @@
         <v>536363520.5</v>
       </c>
       <c r="L66" s="1">
-        <v>47.867528</v>
+        <v>50.960827999999999</v>
       </c>
       <c r="M66" s="1">
-        <v>382940223</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+        <v>407686620.5</v>
+      </c>
+      <c r="N66" s="1">
+        <v>45.757987999999997</v>
+      </c>
+      <c r="O66" s="1">
+        <v>366063906.5</v>
+      </c>
+      <c r="Q66" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B67" s="1">
         <v>151.39014800000001</v>
@@ -3420,29 +3488,338 @@
         <v>288918979.5</v>
       </c>
       <c r="L67" s="1">
-        <v>20.876218000000001</v>
+        <v>21.993981000000002</v>
       </c>
       <c r="M67" s="1">
-        <v>167009744</v>
+        <v>175951846</v>
+      </c>
+      <c r="N67" s="1">
+        <v>18.998203</v>
+      </c>
+      <c r="O67" s="1">
+        <v>151985624.5</v>
+      </c>
+      <c r="Q67" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H68" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L69" s="1">
+        <v>138358.071375</v>
+      </c>
+      <c r="M69" s="1">
+        <v>1106864571002</v>
+      </c>
+      <c r="N69" s="1">
+        <v>136311.46108099999</v>
+      </c>
+      <c r="O69" s="1">
+        <v>1090491688645</v>
+      </c>
+      <c r="Q69" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L70" s="1">
+        <v>21.489221000000001</v>
+      </c>
+      <c r="M70" s="1">
+        <v>171913765</v>
+      </c>
+      <c r="N70" s="1">
+        <v>17.734165000000001</v>
+      </c>
+      <c r="O70" s="1">
+        <v>141873322</v>
+      </c>
+      <c r="Q70" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L71" s="1">
+        <v>260.47150799999997</v>
+      </c>
+      <c r="M71" s="1">
+        <v>2083772060.5</v>
+      </c>
+      <c r="N71" s="1">
+        <v>51.112361999999997</v>
+      </c>
+      <c r="O71" s="1">
+        <v>408898897.5</v>
+      </c>
+      <c r="Q71" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L72" s="1">
+        <v>1.9895620000000001</v>
+      </c>
+      <c r="M72" s="1">
+        <v>15916498</v>
+      </c>
+      <c r="N72" s="1">
+        <v>3.3670550000000001</v>
+      </c>
+      <c r="O72" s="1">
+        <v>26936437.5</v>
+      </c>
+      <c r="Q72" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B112" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
+      <c r="E112" s="11"/>
+      <c r="F112" s="11"/>
+      <c r="G112" s="11"/>
+      <c r="H112" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I112" s="11"/>
+      <c r="J112" s="11"/>
+      <c r="K112" s="11"/>
+      <c r="L112" s="11"/>
+      <c r="M112" s="11"/>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B113" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E113" s="11"/>
+      <c r="F113" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G113" s="11"/>
+      <c r="H113" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I113" s="11"/>
+      <c r="J113" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K113" s="11"/>
+      <c r="L113" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="M113" s="11"/>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B114" s="1">
+        <v>195068.773426</v>
+      </c>
+      <c r="C114" s="1">
+        <v>1560550187406.5</v>
+      </c>
+      <c r="D114" s="1">
+        <v>195197.94776899999</v>
+      </c>
+      <c r="E114" s="1">
+        <v>1561583582150.5</v>
+      </c>
+      <c r="F114" s="1">
+        <v>195434.63178</v>
+      </c>
+      <c r="G114" s="1">
+        <v>1563477054238</v>
+      </c>
+      <c r="H114" s="1">
+        <v>182232.24763100001</v>
+      </c>
+      <c r="I114" s="1">
+        <v>1457857981046</v>
+      </c>
+      <c r="J114" s="1">
+        <v>181947.11027199999</v>
+      </c>
+      <c r="K114" s="1">
+        <v>1455576882174</v>
+      </c>
+      <c r="L114" s="1">
+        <v>181720.94249099999</v>
+      </c>
+      <c r="M114" s="1">
+        <v>1453767539927.5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B115" s="1">
+        <v>118.466221</v>
+      </c>
+      <c r="C115" s="1">
+        <v>947729770</v>
+      </c>
+      <c r="D115" s="1">
+        <v>111.177358</v>
+      </c>
+      <c r="E115" s="1">
+        <v>889418862</v>
+      </c>
+      <c r="F115" s="1">
+        <v>112.174053</v>
+      </c>
+      <c r="G115" s="1">
+        <v>897392426.5</v>
+      </c>
+      <c r="H115" s="1">
+        <v>122.027096</v>
+      </c>
+      <c r="I115" s="1">
+        <v>976216772</v>
+      </c>
+      <c r="J115" s="1">
+        <v>113.205917</v>
+      </c>
+      <c r="K115" s="1">
+        <v>905647335.5</v>
+      </c>
+      <c r="L115" s="1">
+        <v>116.306106</v>
+      </c>
+      <c r="M115" s="1">
+        <v>930448849.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B116" s="1">
+        <v>202.46380300000001</v>
+      </c>
+      <c r="C116" s="1">
+        <v>1619710422</v>
+      </c>
+      <c r="D116" s="1">
+        <v>213.030585</v>
+      </c>
+      <c r="E116" s="1">
+        <v>1704244676</v>
+      </c>
+      <c r="F116" s="1">
+        <v>242.602216</v>
+      </c>
+      <c r="G116" s="1">
+        <v>1940817726.5</v>
+      </c>
+      <c r="H116" s="1">
+        <v>36.531300000000002</v>
+      </c>
+      <c r="I116" s="1">
+        <v>292250400.5</v>
+      </c>
+      <c r="J116" s="1">
+        <v>46.082042000000001</v>
+      </c>
+      <c r="K116" s="1">
+        <v>368656335.5</v>
+      </c>
+      <c r="L116" s="1">
+        <v>54.025700999999998</v>
+      </c>
+      <c r="M116" s="1">
+        <v>432205611</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117" s="1">
+        <v>167.27607399999999</v>
+      </c>
+      <c r="C117" s="1">
+        <v>1338208588.5</v>
+      </c>
+      <c r="D117" s="1">
+        <v>164.59176600000001</v>
+      </c>
+      <c r="E117" s="1">
+        <v>1316734128</v>
+      </c>
+      <c r="F117" s="1">
+        <v>189.06697199999999</v>
+      </c>
+      <c r="G117" s="1">
+        <v>1512535774.5</v>
+      </c>
+      <c r="H117" s="1">
+        <v>14.793008</v>
+      </c>
+      <c r="I117" s="1">
+        <v>118344060.5</v>
+      </c>
+      <c r="J117" s="1">
+        <v>10.728298000000001</v>
+      </c>
+      <c r="K117" s="1">
+        <v>85826388</v>
+      </c>
+      <c r="L117" s="1">
+        <v>12.151139000000001</v>
+      </c>
+      <c r="M117" s="1">
+        <v>97209115.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F118" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="L62:M62"/>
-    <mergeCell ref="J61:M61"/>
+  <mergeCells count="24">
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="J61:O61"/>
+    <mergeCell ref="N62:O62"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="F24:G24"/>
+    <mergeCell ref="L62:M62"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="F113:G113"/>
+    <mergeCell ref="H113:I113"/>
+    <mergeCell ref="J113:K113"/>
+    <mergeCell ref="L113:M113"/>
+    <mergeCell ref="B112:G112"/>
+    <mergeCell ref="H112:M112"/>
     <mergeCell ref="J62:K62"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="D62:E62"/>
     <mergeCell ref="F62:G62"/>
     <mergeCell ref="H62:I62"/>
     <mergeCell ref="B61:E61"/>
-    <mergeCell ref="F61:I61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Clarify the experimental setup
</commit_message>
<xml_diff>
--- a/postgres.xlsx
+++ b/postgres.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xdong\OneDrive\Paper\git_hub\shared_ptp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/29e1f5b82a02f9e3/Paper/git_hub/shared_ptp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_B1CF9780C377B6EE0174307E9F6E61CCA098CD3F" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{8501380F-6DA1-431B-9C6C-94C149E2FC1F}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="11_B1CF9780C377B6EE0174307E9F6E61CCA098CD3F" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{AAA28427-89C1-49E1-92F4-DC293B3D590D}"/>
   <bookViews>
     <workbookView xWindow="923" yWindow="458" windowWidth="24683" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,6 +30,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="176">
   <si>
     <t>CPU_CLK_UNHALTED.THREAD_P</t>
   </si>
@@ -565,6 +566,9 @@
   </si>
   <si>
     <t>CPU_CLK_UNHALTED.THREAD_P (os + usr)</t>
+  </si>
+  <si>
+    <t>select only, the default mode (not reconnect mode)</t>
   </si>
 </sst>
 </file>
@@ -685,6 +689,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -693,9 +700,6 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -989,7 +993,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1010,6 +1014,11 @@
         <v>164</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+    </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>170</v>
@@ -1020,20 +1029,20 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B6" s="21" t="s">
+    <row r="6" spans="1:10" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="B6" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="18" t="s">
         <v>172</v>
       </c>
     </row>
@@ -1268,7 +1277,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="18" t="s">
         <v>173</v>
       </c>
       <c r="B24" s="3">
@@ -1311,40 +1320,40 @@
       <c r="A1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="16"/>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="18"/>
+      <c r="E2" s="19"/>
       <c r="F2" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="J2" s="18"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="16" t="s">
         <v>131</v>
       </c>
@@ -2043,40 +2052,40 @@
       <c r="A1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="13"/>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="18"/>
+      <c r="E2" s="19"/>
       <c r="F2" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="J2" s="18"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="13" t="s">
         <v>131</v>
       </c>
@@ -3445,40 +3454,40 @@
       <c r="A1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="11"/>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="18"/>
+      <c r="E2" s="19"/>
       <c r="F2" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="J2" s="18"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="11" t="s">
         <v>131</v>
       </c>
@@ -5004,18 +5013,18 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" s="2"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19" t="s">
+      <c r="E2" s="20"/>
+      <c r="F2" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="19"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B3" s="4" t="s">
@@ -6569,18 +6578,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="20"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="B2" s="6" t="s">
@@ -6985,18 +6994,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20" t="s">
+      <c r="C24" s="21"/>
+      <c r="D24" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20" t="s">
+      <c r="E24" s="21"/>
+      <c r="F24" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="G24" s="20"/>
+      <c r="G24" s="21"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A25" s="9" t="s">
@@ -7506,62 +7515,62 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A61" s="3"/>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20" t="s">
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="G61" s="20"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="20"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
-      <c r="L61" s="20" t="s">
+      <c r="L61" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="M61" s="20"/>
-      <c r="N61" s="20"/>
-      <c r="O61" s="20"/>
-      <c r="P61" s="20"/>
-      <c r="Q61" s="20"/>
+      <c r="M61" s="21"/>
+      <c r="N61" s="21"/>
+      <c r="O61" s="21"/>
+      <c r="P61" s="21"/>
+      <c r="Q61" s="21"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20" t="s">
+      <c r="C62" s="21"/>
+      <c r="D62" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20" t="s">
+      <c r="E62" s="21"/>
+      <c r="F62" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="G62" s="20"/>
-      <c r="H62" s="20" t="s">
+      <c r="G62" s="21"/>
+      <c r="H62" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="I62" s="20"/>
-      <c r="J62" s="20" t="s">
+      <c r="I62" s="21"/>
+      <c r="J62" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="K62" s="20"/>
-      <c r="L62" s="20" t="s">
+      <c r="K62" s="21"/>
+      <c r="L62" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="M62" s="20"/>
-      <c r="N62" s="20" t="s">
+      <c r="M62" s="21"/>
+      <c r="N62" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="O62" s="20"/>
-      <c r="P62" s="20" t="s">
+      <c r="O62" s="21"/>
+      <c r="P62" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="Q62" s="20"/>
+      <c r="Q62" s="21"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B63" s="6" t="s">
@@ -7959,52 +7968,52 @@
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="B112" s="20" t="s">
+      <c r="B112" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C112" s="20"/>
-      <c r="D112" s="20"/>
-      <c r="E112" s="20"/>
-      <c r="F112" s="20"/>
-      <c r="G112" s="20"/>
-      <c r="H112" s="20" t="s">
+      <c r="C112" s="21"/>
+      <c r="D112" s="21"/>
+      <c r="E112" s="21"/>
+      <c r="F112" s="21"/>
+      <c r="G112" s="21"/>
+      <c r="H112" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="I112" s="20"/>
-      <c r="J112" s="20"/>
-      <c r="K112" s="20"/>
-      <c r="L112" s="20"/>
-      <c r="M112" s="20"/>
-      <c r="N112" s="20"/>
-      <c r="O112" s="20"/>
+      <c r="I112" s="21"/>
+      <c r="J112" s="21"/>
+      <c r="K112" s="21"/>
+      <c r="L112" s="21"/>
+      <c r="M112" s="21"/>
+      <c r="N112" s="21"/>
+      <c r="O112" s="21"/>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="B113" s="20" t="s">
+      <c r="B113" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C113" s="20"/>
-      <c r="D113" s="20" t="s">
+      <c r="C113" s="21"/>
+      <c r="D113" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="E113" s="20"/>
-      <c r="F113" s="20" t="s">
+      <c r="E113" s="21"/>
+      <c r="F113" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="G113" s="20"/>
-      <c r="H113" s="20" t="s">
+      <c r="G113" s="21"/>
+      <c r="H113" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="I113" s="20"/>
+      <c r="I113" s="21"/>
       <c r="J113" s="10"/>
       <c r="K113" s="10"/>
-      <c r="L113" s="20" t="s">
+      <c r="L113" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="M113" s="20"/>
-      <c r="N113" s="20" t="s">
+      <c r="M113" s="21"/>
+      <c r="N113" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="O113" s="20"/>
+      <c r="O113" s="21"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A114" s="1" t="s">
@@ -8177,6 +8186,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="L61:Q61"/>
+    <mergeCell ref="P62:Q62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="N62:O62"/>
+    <mergeCell ref="B61:E61"/>
     <mergeCell ref="N113:O113"/>
     <mergeCell ref="B112:G112"/>
     <mergeCell ref="H112:O112"/>
@@ -8190,18 +8211,6 @@
     <mergeCell ref="F113:G113"/>
     <mergeCell ref="H113:I113"/>
     <mergeCell ref="L113:M113"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="L61:Q61"/>
-    <mergeCell ref="P62:Q62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="N62:O62"/>
-    <mergeCell ref="B61:E61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated postgres.xlsx with parallelism experiment results
</commit_message>
<xml_diff>
--- a/postgres.xlsx
+++ b/postgres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/29e1f5b82a02f9e3/Paper/git_hub/shared_ptp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="11_B1CF9780C377B6EE0174307E9F6E61CCA098CD3F" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{AAA28427-89C1-49E1-92F4-DC293B3D590D}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="11_B1CF9780C377B6EE0174307E9F6E61CCA098CD3F" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{B3491376-B00D-42A6-AE1D-3C11ADF2C06F}"/>
   <bookViews>
     <workbookView xWindow="923" yWindow="458" windowWidth="24683" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="176">
   <si>
     <t>CPU_CLK_UNHALTED.THREAD_P</t>
   </si>
@@ -544,9 +544,6 @@
     <t>INST_RETIRED.ANY_P (os + user)</t>
   </si>
   <si>
-    <t>4 clients</t>
-  </si>
-  <si>
     <t>16 clients</t>
   </si>
   <si>
@@ -556,12 +553,6 @@
     <t>all results presented are per transaction per client and are user-space results  (3,000,000 transactions per client)</t>
   </si>
   <si>
-    <t>16 clients/ 4 clients</t>
-  </si>
-  <si>
-    <t>32 clients/ 4 clients</t>
-  </si>
-  <si>
     <t>inst addr translation overhead / total execution cycles</t>
   </si>
   <si>
@@ -569,6 +560,15 @@
   </si>
   <si>
     <t>select only, the default mode (not reconnect mode)</t>
+  </si>
+  <si>
+    <t>32 clients/ 16 clients</t>
+  </si>
+  <si>
+    <t>Ms_L (main executable mapped by superpages)</t>
+  </si>
+  <si>
+    <t>Msp_L (main executable padded and mapped by superpages)</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -626,6 +626,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -662,7 +669,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1"/>
@@ -701,6 +708,8 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma" xfId="5" builtinId="3"/>
@@ -990,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B98BA9-6D5F-43A5-B1C1-4803FF720BC6}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1004,196 +1013,190 @@
     <col min="10" max="10" width="13.8125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A5" s="22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B6" s="18" t="s">
         <v>167</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>169</v>
-      </c>
       <c r="I6" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="3">
-        <v>139320.31380500001</v>
+        <v>165743.07998499999</v>
       </c>
       <c r="C7" s="3">
-        <v>166233.025177</v>
+        <v>182013.945997</v>
       </c>
       <c r="I7" s="3">
         <f>C7/B7</f>
-        <v>1.1931714811500385</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+        <v>1.0981692026808754</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>30.529081000000001</v>
+        <v>244.463626</v>
       </c>
       <c r="C8" s="3">
-        <v>245.57641899999999</v>
+        <v>272.06217400000003</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" ref="I8:I21" si="0">C8/B8</f>
-        <v>8.0440160973073507</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
+        <v>1.1128942920939904</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="3">
-        <v>1641.985588</v>
+        <v>10593.21163</v>
       </c>
       <c r="C9" s="3">
-        <v>10657.799916</v>
+        <v>13124.108267</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" si="0"/>
-        <v>6.4907999155958489</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+        <v>1.238916838953023</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="3">
-        <v>1.9639869999999999</v>
+        <v>22.719802000000001</v>
       </c>
       <c r="C10" s="3">
-        <v>22.867788999999998</v>
+        <v>25.990590999999998</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="0"/>
-        <v>11.643554157945037</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
+        <v>1.1439620380494511</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3">
-        <v>244.754627</v>
+        <v>1137.7385899999999</v>
       </c>
       <c r="C11" s="3">
-        <v>1127.1537330000001</v>
+        <v>1441.553637</v>
       </c>
       <c r="I11" s="3">
         <f t="shared" si="0"/>
-        <v>4.6052397326077932</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
+        <v>1.2670341409444503</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="3">
-        <v>112.59295400000001</v>
+        <v>354.86586599999998</v>
       </c>
       <c r="C12" s="3">
-        <v>351.782555</v>
+        <v>381.56842</v>
       </c>
       <c r="I12" s="3">
         <f t="shared" si="0"/>
-        <v>3.124374505708412</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+        <v>1.0752468934276143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="3">
-        <v>4846.5346250000002</v>
+        <v>13146.213442</v>
       </c>
       <c r="C13" s="3">
-        <v>13019.730836000001</v>
+        <v>15158.517922000001</v>
       </c>
       <c r="I13" s="3">
         <f t="shared" si="0"/>
-        <v>2.6864000452694587</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A14" t="s">
+        <v>1.1530710336385546</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A14" s="23" t="s">
         <v>145</v>
       </c>
       <c r="B14" s="3">
-        <v>14025.579484</v>
+        <v>24734.480510000001</v>
       </c>
       <c r="C14" s="3">
-        <v>24380.117581999999</v>
+        <v>28882.239214000001</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="0"/>
-        <v>1.738260983071122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+        <v>1.1676913611475723</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B15" s="3">
-        <v>202674.90353099999</v>
+        <v>231668.26772</v>
       </c>
       <c r="C15" s="3">
-        <v>231706.077494</v>
+        <v>242133.400352</v>
       </c>
       <c r="I15" s="3">
         <f t="shared" si="0"/>
-        <v>1.1432401025347452</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+        <v>1.0451729221916937</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>146</v>
       </c>
       <c r="B16" s="3">
-        <v>170226.30035899999</v>
+        <v>155139.899294</v>
       </c>
       <c r="C16" s="3">
-        <v>155138.92887999999</v>
+        <v>150516.268794</v>
       </c>
       <c r="I16" s="3">
         <f t="shared" si="0"/>
-        <v>0.91136874004086699</v>
+        <v>0.97019702525887341</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.5">
@@ -1201,29 +1204,29 @@
         <v>166</v>
       </c>
       <c r="B17" s="3">
-        <v>117670.28529</v>
+        <v>118162.038227</v>
       </c>
       <c r="C17" s="3">
-        <v>118168.297143</v>
+        <v>118790.674011</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="0"/>
-        <v>1.0042322651956919</v>
+        <v>1.0053201162863519</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A18" t="s">
+      <c r="A18" s="23" t="s">
         <v>136</v>
       </c>
       <c r="B18" s="3">
-        <v>4251.3366150000002</v>
+        <v>5722.9740410000004</v>
       </c>
       <c r="C18" s="3">
-        <v>5553.3820040000001</v>
+        <v>13366.601137</v>
       </c>
       <c r="I18" s="3">
         <f t="shared" si="0"/>
-        <v>1.3062673005957679</v>
+        <v>2.3356040130953302</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.5">
@@ -1231,14 +1234,14 @@
         <v>137</v>
       </c>
       <c r="B19" s="3">
-        <v>37353.777627000003</v>
+        <v>50889.468272999999</v>
       </c>
       <c r="C19" s="3">
-        <v>51099.054978</v>
+        <v>62655.917521000003</v>
       </c>
       <c r="I19" s="3">
         <f t="shared" si="0"/>
-        <v>1.3679755629605894</v>
+        <v>1.2312158025483404</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.5">
@@ -1246,14 +1249,14 @@
         <v>134</v>
       </c>
       <c r="B20" s="3">
-        <v>19332.581488</v>
+        <v>31178.224119999999</v>
       </c>
       <c r="C20" s="3">
-        <v>31366.939052999998</v>
+        <v>43034.913572999998</v>
       </c>
       <c r="I20" s="3">
         <f t="shared" si="0"/>
-        <v>1.6224909783760586</v>
+        <v>1.3802875175752634</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.5">
@@ -1261,36 +1264,585 @@
         <v>135</v>
       </c>
       <c r="B21" s="3">
-        <v>15235.831464000001</v>
+        <v>24607.062817000002</v>
       </c>
       <c r="C21" s="3">
-        <v>24829.723055999999</v>
+        <v>35506.512418999999</v>
       </c>
       <c r="I21" s="3">
         <f t="shared" si="0"/>
-        <v>1.6296926829801797</v>
+        <v>1.4429398861236709</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>147</v>
       </c>
+      <c r="B22" s="3">
+        <v>0.55557599999999996</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2.1887E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A24" s="18" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B24" s="3">
         <f>B14/B7</f>
-        <v>0.1006714606143576</v>
+        <v>0.1492338655239091</v>
       </c>
       <c r="C24" s="3">
         <f>C14/C7</f>
-        <v>0.1466622986379558</v>
+        <v>0.15868146287249904</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A26" s="22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="3">
+        <v>152574.461262</v>
+      </c>
+      <c r="C28" s="3">
+        <v>166649.42162499999</v>
+      </c>
+      <c r="I28" s="3">
+        <f>C28/B28</f>
+        <v>1.0922497792001411</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="3">
+        <v>218.303101</v>
+      </c>
+      <c r="C29" s="3">
+        <v>240.19660099999999</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" ref="I29:I42" si="1">C29/B29</f>
+        <v>1.1002894594703903</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="3">
+        <v>9655.7835930000001</v>
+      </c>
+      <c r="C30" s="3">
+        <v>11703.143278</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="1"/>
+        <v>1.2120345454390922</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="3">
+        <v>19.670846000000001</v>
+      </c>
+      <c r="C31" s="3">
+        <v>21.971233999999999</v>
+      </c>
+      <c r="I31" s="3">
+        <f t="shared" si="1"/>
+        <v>1.1169440297585573</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1013.05911</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1267.1822299999999</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" si="1"/>
+        <v>1.2508472778059316</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="3">
+        <v>61.573349</v>
+      </c>
+      <c r="C33" s="3">
+        <v>63.293998000000002</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0279447038035887</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="3">
+        <v>3204.627954</v>
+      </c>
+      <c r="C34" s="3">
+        <v>3683.725817</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" si="1"/>
+        <v>1.1495018672610631</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A35" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B35" s="3">
+        <v>6993.5675099999999</v>
+      </c>
+      <c r="C35" s="3">
+        <v>7385.6365919999998</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0560613851856562</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
+        <v>171</v>
+      </c>
+      <c r="B36" s="3">
+        <v>217409.398602</v>
+      </c>
+      <c r="C36" s="3">
+        <v>225768.40391299999</v>
+      </c>
+      <c r="I36" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0384482242476665</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37" s="3">
+        <v>154977.76902499999</v>
+      </c>
+      <c r="C37" s="3">
+        <v>150416.98414099999</v>
+      </c>
+      <c r="I37" s="3">
+        <f t="shared" si="1"/>
+        <v>0.97057136057195226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
+        <v>166</v>
+      </c>
+      <c r="B38" s="3">
+        <v>118162.55101900001</v>
+      </c>
+      <c r="C38" s="3">
+        <v>118709.855757</v>
+      </c>
+      <c r="I38" s="3">
+        <f t="shared" si="1"/>
+        <v>1.004631795211598</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A39" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B39" s="3">
+        <v>5594.9140040000002</v>
+      </c>
+      <c r="C39" s="3">
+        <v>12147.400122999999</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" si="1"/>
+        <v>2.1711504617077932</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A40" t="s">
+        <v>137</v>
+      </c>
+      <c r="B40" s="3">
+        <v>48266.559349000003</v>
+      </c>
+      <c r="C40" s="3">
+        <v>57211.711948999997</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" si="1"/>
+        <v>1.1853281593021883</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="3">
+        <v>27533.973085000001</v>
+      </c>
+      <c r="C41" s="3">
+        <v>35862.757570000002</v>
+      </c>
+      <c r="I41" s="3">
+        <f t="shared" si="1"/>
+        <v>1.3024911973033551</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A42" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" s="3">
+        <v>22119.370794999999</v>
+      </c>
+      <c r="C42" s="3">
+        <v>29747.440600000002</v>
+      </c>
+      <c r="I42" s="3">
+        <f t="shared" si="1"/>
+        <v>1.3448592582355146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0.55942400000000003</v>
+      </c>
+      <c r="C43" s="3">
+        <v>5.4174E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A45" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B45" s="3">
+        <f>B35/B28</f>
+        <v>4.5837078185651831E-2</v>
+      </c>
+      <c r="C45" s="3">
+        <f>C35/C28</f>
+        <v>4.4318405188464451E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A47" s="22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="3">
+        <v>150794.91561600001</v>
+      </c>
+      <c r="C49" s="3">
+        <v>162108.05302299999</v>
+      </c>
+      <c r="I49" s="3">
+        <f>C49/B49</f>
+        <v>1.0750233345785274</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="3">
+        <v>115.18022499999999</v>
+      </c>
+      <c r="C50" s="3">
+        <v>121.94078399999999</v>
+      </c>
+      <c r="I50" s="3">
+        <f t="shared" ref="I50:I63" si="2">C50/B50</f>
+        <v>1.0586954835346085</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="3">
+        <v>5726.2879899999998</v>
+      </c>
+      <c r="C51" s="3">
+        <v>6986.4605460000002</v>
+      </c>
+      <c r="I51" s="3">
+        <f t="shared" si="2"/>
+        <v>1.2200679669273848</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="3">
+        <v>18.575039</v>
+      </c>
+      <c r="C52" s="3">
+        <v>20.058209000000002</v>
+      </c>
+      <c r="I52" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0798474770362529</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" s="3">
+        <v>934.029088</v>
+      </c>
+      <c r="C53" s="3">
+        <v>1173.958883</v>
+      </c>
+      <c r="I53" s="3">
+        <f t="shared" si="2"/>
+        <v>1.2568761488079052</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="3">
+        <v>52.038491999999998</v>
+      </c>
+      <c r="C54" s="3">
+        <v>51.612158000000001</v>
+      </c>
+      <c r="I54" s="3">
+        <f t="shared" si="2"/>
+        <v>0.99180733369445073</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="3">
+        <v>2709.4517139999998</v>
+      </c>
+      <c r="C55" s="3">
+        <v>3113.1937389999998</v>
+      </c>
+      <c r="I55" s="3">
+        <f t="shared" si="2"/>
+        <v>1.149012445179896</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A56" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" s="3">
+        <v>6477.8670060000004</v>
+      </c>
+      <c r="C56" s="3">
+        <v>7214.6310800000001</v>
+      </c>
+      <c r="I56" s="3">
+        <f t="shared" si="2"/>
+        <v>1.1137355974300778</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A57" t="s">
+        <v>171</v>
+      </c>
+      <c r="B57" s="3">
+        <v>216587.29824199999</v>
+      </c>
+      <c r="C57" s="3">
+        <v>221691.1023</v>
+      </c>
+      <c r="I57" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0235646508332976</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A58" t="s">
+        <v>146</v>
+      </c>
+      <c r="B58" s="3">
+        <v>155293.896614</v>
+      </c>
+      <c r="C58" s="3">
+        <v>150259.353775</v>
+      </c>
+      <c r="I58" s="3">
+        <f t="shared" si="2"/>
+        <v>0.96758054921170589</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A59" t="s">
+        <v>166</v>
+      </c>
+      <c r="B59" s="3">
+        <v>118161.723644</v>
+      </c>
+      <c r="C59" s="3">
+        <v>118684.761117</v>
+      </c>
+      <c r="I59" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0044264543277637</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A60" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="3">
+        <v>5730.3346369999999</v>
+      </c>
+      <c r="C60" s="3">
+        <v>11120.157907999999</v>
+      </c>
+      <c r="I60" s="3">
+        <f t="shared" si="2"/>
+        <v>1.9405774029667719</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A61" t="s">
+        <v>137</v>
+      </c>
+      <c r="B61" s="3">
+        <v>45948.709331999999</v>
+      </c>
+      <c r="C61" s="3">
+        <v>54975.398408000001</v>
+      </c>
+      <c r="I61" s="3">
+        <f t="shared" si="2"/>
+        <v>1.1964514174006093</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A62" t="s">
+        <v>134</v>
+      </c>
+      <c r="B62" s="3">
+        <v>26041.050367</v>
+      </c>
+      <c r="C62" s="3">
+        <v>34503.573315000001</v>
+      </c>
+      <c r="I62" s="3">
+        <f t="shared" si="2"/>
+        <v>1.324968571879265</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A63" t="s">
+        <v>135</v>
+      </c>
+      <c r="B63" s="3">
+        <v>20931.854705000002</v>
+      </c>
+      <c r="C63" s="3">
+        <v>28757.293478</v>
+      </c>
+      <c r="I63" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3738531001331062</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A64" t="s">
+        <v>147</v>
+      </c>
+      <c r="B64" s="3">
+        <v>0.56265699999999996</v>
+      </c>
+      <c r="C64" s="3">
+        <v>8.1216999999999998E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A66" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B66" s="3">
+        <f>B56/B49</f>
+        <v>4.2958126137992082E-2</v>
+      </c>
+      <c r="C66" s="3">
+        <f>C56/C49</f>
+        <v>4.4505075136374528E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1298,7 +1850,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
@@ -2003,6 +2557,16 @@
       <c r="K23" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B24" s="1">
+        <f>B22/B4</f>
+        <v>0.11581447083429915</v>
+      </c>
+      <c r="D24" s="1">
+        <f>D22/D4</f>
+        <v>1.8735191919936969E-2</v>
       </c>
     </row>
     <row r="41" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.5">

</xml_diff>